<commit_message>
Add dictionary upload v2, parse xlsx itself, avoid mount path with mc
</commit_message>
<xml_diff>
--- a/module/admin-api/InitFiles/wordbank_template.xlsx
+++ b/module/admin-api/InitFiles/wordbank_template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changmin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/workspaces/go-dev/emotigo/module/admin-api/InitFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{521A092A-64B3-C746-A285-393B4260F5B1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="示例" sheetId="2" r:id="rId1"/>
     <sheet name="词库模板" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -271,7 +272,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -346,6 +347,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1455,14 +1459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1698,14 +1702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
UPDATE: Update template file of wordbank
</commit_message>
<xml_diff>
--- a/module/admin-api/InitFiles/wordbank_template.xlsx
+++ b/module/admin-api/InitFiles/wordbank_template.xlsx
@@ -1,46 +1,138 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/workspaces/go-dev/emotigo/module/admin-api/InitFiles/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{437BCAA7-C17F-C54B-850B-DB6CB54E924E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25780" windowHeight="16300" tabRatio="204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25785" windowHeight="16305" tabRatio="204"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="1" r:id="rId1"/>
     <sheet name="例子" sheetId="2" r:id="rId2"/>
     <sheet name="词库模板" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
-  <si>
-    <t>1.excel导入文件：
- - 请在excel导入文件的“词库模板”sheet页，填写所有词库内容，请勿修改第一行名称，否则无法读取
- - excel文件中，若词语和同义词两列均为空，则系统不对导入文件做检测
- - excel文件中，若词语或同义词两列中有内容，则词库导入后，会将此次导入之前的词库内容全部替换，请谨慎检查
-2.目录：
- - 一级目录有且只有两个，名称分别为：敏感词库、专有词库。请勿修改一级目录名称
- - 当一个父目录包含几个子目录时，表格中不需要在不同行多次填写父目录名称，只需要在第一个子目录的同一行填写一次
- - 目录之间不可有空白目录列。例如一级目录、二级目录、四级目录有内容，三级目录为空 —&gt; 上传后会报错
- - 目录字数限制：1~20字
-3.词语：
- - 词语字数限制：1~35字</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+  <si>
+    <t>一级目录</t>
+  </si>
+  <si>
+    <t>二级目录</t>
+  </si>
+  <si>
+    <t>三级目录</t>
+  </si>
+  <si>
+    <t>四级目录</t>
+  </si>
+  <si>
+    <t>词语</t>
+  </si>
+  <si>
+    <t>同义词</t>
+  </si>
+  <si>
+    <t>敏感词库</t>
+  </si>
+  <si>
+    <t>敏感词分类1</t>
+  </si>
+  <si>
+    <t>敏感词分类1-1</t>
+  </si>
+  <si>
+    <t>敏感词分类1-1-1</t>
+  </si>
+  <si>
+    <t>政治1</t>
+  </si>
+  <si>
+    <t>一一，二二</t>
+  </si>
+  <si>
+    <t>政治2</t>
+  </si>
+  <si>
+    <t>三三，四四</t>
+  </si>
+  <si>
+    <t>敏感词分类1-2</t>
+  </si>
+  <si>
+    <t>色情</t>
+  </si>
+  <si>
+    <t>五五，六六，七七，八八</t>
+  </si>
+  <si>
+    <t>专有词库</t>
+  </si>
+  <si>
+    <t>乐蜂专用</t>
+  </si>
+  <si>
+    <t>防伪码</t>
+  </si>
+  <si>
+    <t>防伪码，真品码，防伪，防伪标识，防伪标，防伪标志</t>
+  </si>
+  <si>
+    <t>唯品会专用</t>
+  </si>
+  <si>
+    <t>其他分类</t>
+  </si>
+  <si>
+    <t>活动类</t>
+  </si>
+  <si>
+    <t>通用同义词</t>
+  </si>
+  <si>
+    <t>名词</t>
+  </si>
+  <si>
+    <t>小孩</t>
+  </si>
+  <si>
+    <t>BABY，儿童，娃，娃娃，婴儿，婴幼儿，孩子，宝宝，小孩子，小盆友，小朋友</t>
+  </si>
+  <si>
+    <t>尺码表</t>
+  </si>
+  <si>
+    <t>尺码参照，尺码对比表，尺码对照表，码数表</t>
+  </si>
+  <si>
+    <t>奶瓶</t>
+  </si>
+  <si>
+    <t>不锈钢奶瓶，塑料奶瓶，奶瓶</t>
+  </si>
+  <si>
+    <t>动词</t>
+  </si>
+  <si>
+    <t>看</t>
+  </si>
+  <si>
+    <t>瞧，望，瞅，瞄</t>
+  </si>
+  <si>
+    <t>卖</t>
+  </si>
+  <si>
+    <t>形容词</t>
   </si>
   <si>
     <t>4.同义词：
  - 一组词需填写在“同义词”列的同一单元格中，使用逗号分隔
- - 同义词单元格字数限制：1~5000字（包括符号）
- - 每个词的字数限制：1~35字
+ - 同义词单元格字数限制：1~32767字（包括符号）
+ - 每个词的字数限制：1~64字
  - 词语加所有同义词，总数不超过10000个
  - 词语和同义词不可以均为空
 5.其他：
@@ -48,123 +140,44 @@
  - 如果同义词单元格中有内容，词语对应单元格的内容不可以为空；即同义词必须属于某个词库
  - 如果同义词单元格中无内容，二级目录、三级目录、四级目录和词语都可以为空；即只有分类结构，分类目录中没有词
  - 同义词中的每个词是系统最终识别的对象，词语和目录仅是分类名称。如需系统识别词语或者目录名，请将这些名称也填入同义词单元格中</t>
-  </si>
-  <si>
-    <t>一级目录</t>
-  </si>
-  <si>
-    <t>二级目录</t>
-  </si>
-  <si>
-    <t>三级目录</t>
-  </si>
-  <si>
-    <t>四级目录</t>
-  </si>
-  <si>
-    <t>词语</t>
-  </si>
-  <si>
-    <t>同义词</t>
-  </si>
-  <si>
-    <t>敏感词库</t>
-  </si>
-  <si>
-    <t>敏感词分类1</t>
-  </si>
-  <si>
-    <t>敏感词分类1-1</t>
-  </si>
-  <si>
-    <t>敏感词分类1-1-1</t>
-  </si>
-  <si>
-    <t>政治1</t>
-  </si>
-  <si>
-    <t>一一，二二</t>
-  </si>
-  <si>
-    <t>政治2</t>
-  </si>
-  <si>
-    <t>三三，四四</t>
-  </si>
-  <si>
-    <t>敏感词分类1-2</t>
-  </si>
-  <si>
-    <t>色情</t>
-  </si>
-  <si>
-    <t>五五，六六，七七，八八</t>
-  </si>
-  <si>
-    <t>专有词库</t>
-  </si>
-  <si>
-    <t>乐蜂专用</t>
-  </si>
-  <si>
-    <t>防伪码</t>
-  </si>
-  <si>
-    <t>防伪码，真品码，防伪，防伪标识，防伪标，防伪标志</t>
-  </si>
-  <si>
-    <t>唯品会专用</t>
-  </si>
-  <si>
-    <t>其他分类</t>
-  </si>
-  <si>
-    <t>活动类</t>
-  </si>
-  <si>
-    <t>通用同义词</t>
-  </si>
-  <si>
-    <t>名词</t>
-  </si>
-  <si>
-    <t>小孩</t>
-  </si>
-  <si>
-    <t>BABY，儿童，娃，娃娃，婴儿，婴幼儿，孩子，宝宝，小孩子，小盆友，小朋友</t>
-  </si>
-  <si>
-    <t>尺码表</t>
-  </si>
-  <si>
-    <t>尺码参照，尺码对比表，尺码对照表，码数表</t>
-  </si>
-  <si>
-    <t>奶瓶</t>
-  </si>
-  <si>
-    <t>不锈钢奶瓶，塑料奶瓶，奶瓶</t>
-  </si>
-  <si>
-    <t>动词</t>
-  </si>
-  <si>
-    <t>看</t>
-  </si>
-  <si>
-    <t>瞧，望，瞅，瞄</t>
-  </si>
-  <si>
-    <t>卖</t>
-  </si>
-  <si>
-    <t>形容词</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务引擎词库</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*敏感词库</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*专有词库</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*任务引擎词库</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.excel导入文件：
+ - 请在excel导入文件的“词库模板”sheet页，填写所有词库内容，请勿修改第一行名称，否则无法读取
+ - excel文件中，若词语和同义词两列均为空，则系统不对导入文件做检测
+ - excel文件中，若词语或同义词两列中有内容，则词库导入后，会将此次导入之前的词库内容全部替换，请谨慎检查
+2.目录：
+ - 一级目录有三个特定名称，分别为：敏感词库、专有词库、任务引擎词库。请勿修改保留目录名称
+ - 当一个父目录包含几个子目录时，表格中不需要在不同行多次填写父目录名称，只需要在第一个子目录的同一行填写一次
+ - 目录之间不可有空白目录列。例如一级目录、二级目录、四级目录有内容，三级目录为空 —&gt; 上传后会报错
+ - 目录字数限制：1~20字
+ - 目录名称可使用 * 开头，导入后 * 符号不会出现，且导入后该目录名称不可修改
+3.词语：
+ - 词语字数限制：1~35字</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -584,26 +597,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="143.796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="124.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="201" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="238">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -618,154 +629,161 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="5" width="20.796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="80.796875" style="2" customWidth="1"/>
+    <col min="1" max="5" width="20.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="80.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="E9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -781,44 +799,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="5" width="20.796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="80.796875" style="2" customWidth="1"/>
+    <col min="1" max="5" width="20.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="80.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.95" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>